<commit_message>
Correct typo in Excel XSD/XML
</commit_message>
<xml_diff>
--- a/data/inventoryData.xlsx
+++ b/data/inventoryData.xlsx
@@ -518,7 +518,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema2">
+  <Schema ID="Schema3">
     <xs:schema xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns="">
       <!-- define strings -->
       <xs:simpleType name="stringType">
@@ -526,7 +526,7 @@
       </xs:simpleType>
       <!-- define integers -->
       <xs:simpleType name="intType">
-        <xs:restriction base="xs:positiveInteger"/>
+        <xs:restriction base="xs:integer"/>
       </xs:simpleType>
       <!-- define a product -->
       <xs:complexType name="productType">
@@ -563,14 +563,14 @@
       <!-- define an inventory -->
       <xs:complexType name="inventoryType">
         <xs:sequence>
-          <xs:element name="producty" type="productType" minOccurs="1" maxOccurs="unbounded"/>
+          <xs:element name="product" type="productType" minOccurs="1" maxOccurs="unbounded"/>
         </xs:sequence>
       </xs:complexType>
       <!-- define the root -->
       <xs:element name="inventory" type="inventoryType"/>
     </xs:schema>
   </Schema>
-  <Map ID="4" Name="inventory_Map" RootElement="inventory" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="5" Name="inventory_Map" RootElement="inventory" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
@@ -579,86 +579,86 @@
   <autoFilter ref="A1:AA28"/>
   <tableColumns count="27">
     <tableColumn id="1" uniqueName="description" name="Item Description " dataDxfId="23">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/description" xmlDataType="string"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/description" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="minQuantity" name="Min. Quant." dataDxfId="22">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/minQuantity" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/minQuantity" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="week1" name="W1" dataDxfId="21">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week1" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week1" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="week2" name="W2" dataDxfId="20">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week2" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week2" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="week3" name="W3" dataDxfId="19">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week3" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week3" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="week4" name="W4" dataDxfId="18">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week4" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week4" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="week5" name="W5" dataDxfId="17">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week5" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week5" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="8" uniqueName="week6" name="W6" dataDxfId="16">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week6" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week6" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="9" uniqueName="week7" name="W7" dataDxfId="15">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week7" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week7" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="10" uniqueName="week8" name="W8" dataDxfId="14">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week8" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week8" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="11" uniqueName="week9" name="W9" dataDxfId="13">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week9" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week9" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="12" uniqueName="week10" name="W10" dataDxfId="12">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week10" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week10" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="13" uniqueName="week11" name="W11" dataDxfId="11">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week11" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week11" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="14" uniqueName="week12" name="W12" dataDxfId="10">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week12" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week12" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="15" uniqueName="week13" name="W13" dataDxfId="9">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week13" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week13" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="16" uniqueName="week14" name="W14" dataDxfId="8">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week14" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week14" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="17" uniqueName="week15" name="W15" dataDxfId="7">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week15" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week15" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="18" uniqueName="week16" name="W16" dataDxfId="6">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week16" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week16" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="19" uniqueName="week17" name="W17" dataDxfId="5">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week17" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week17" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="20" uniqueName="week18" name="W18" dataDxfId="4">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week18" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week18" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="21" uniqueName="week19" name="W19" dataDxfId="3">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week19" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week19" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="22" uniqueName="week20" name="W20" dataDxfId="2">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/week20" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/week20" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="23" uniqueName="salesTotal" name="Sales 20WTot">
       <calculatedColumnFormula>SUM(C2:V2)</calculatedColumnFormula>
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/salesTotal" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/salesTotal" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="24" uniqueName="marketAPS" name="Mkt APS" dataDxfId="1">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/marketAPS" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/marketAPS" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="25" uniqueName="numStores" name="# of Strs" dataDxfId="0">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/numStores" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/numStores" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="26" uniqueName="monthlySales" name="Monthly Sales">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/monthlySales" xmlDataType="positiveInteger"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/monthlySales" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="27" uniqueName="currentPromotion" name="Current Promotions">
-      <xmlColumnPr mapId="4" xpath="/inventory/producty/currentPromotion" xmlDataType="string"/>
+      <xmlColumnPr mapId="5" xpath="/inventory/product/currentPromotion" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>

</xml_diff>